<commit_message>
al refresh punta a dashboard
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23385" windowHeight="10605" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23385" windowHeight="10605" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GITHUB" sheetId="3" r:id="rId1"/>
-    <sheet name="BUG - Cli-Sea" sheetId="1" r:id="rId2"/>
-    <sheet name="CHANGELOG - CLI-Sea" sheetId="2" r:id="rId3"/>
-    <sheet name="ERROR" sheetId="5" r:id="rId4"/>
+    <sheet name="BUG - Seaoracle" sheetId="1" r:id="rId2"/>
+    <sheet name="TO-FIX Seaoracle" sheetId="6" r:id="rId3"/>
+    <sheet name="CHANGELOG - CLI-Sea" sheetId="2" r:id="rId4"/>
+    <sheet name="ERROR" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
   <si>
     <t>SEZIONE</t>
   </si>
@@ -71,19 +72,10 @@
     <t>NEW VOY: se ne creo uno nuovo ho la possibilità di salvarlo con un NUMBER vuoto</t>
   </si>
   <si>
-    <t>Documenti</t>
-  </si>
-  <si>
-    <t>GENERAZIONE CODICE DOC: funzione custom per la generazione del codice (layout con input group + button get code a cui passo parametri inseriti dall'utente)</t>
-  </si>
-  <si>
     <t>Equipment</t>
   </si>
   <si>
     <t xml:space="preserve">EXEL: import template </t>
-  </si>
-  <si>
-    <t>CANCELLAZIONE: aggiungere un controllo; solo se le leg non hanno un booking associato</t>
   </si>
   <si>
     <t>controllo sulla uniqueKey su tutti i POST</t>
@@ -594,12 +586,18 @@
   <si>
     <t>mettere su 10 elementi</t>
   </si>
+  <si>
+    <t>13/0tt/2014</t>
+  </si>
+  <si>
+    <t>PRIORITY</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -649,8 +647,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -681,8 +703,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -779,11 +806,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -795,7 +838,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -817,6 +859,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -845,10 +899,30 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -930,14 +1004,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E33" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E32" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:E32"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="SEZIONE" dataDxfId="4"/>
-    <tableColumn id="2" name="BUG" dataDxfId="3"/>
-    <tableColumn id="3" name="TO FIX" dataDxfId="2"/>
-    <tableColumn id="4" name="NOTE" dataDxfId="1"/>
-    <tableColumn id="5" name="DATE" dataDxfId="0"/>
+    <tableColumn id="1" name="SEZIONE" dataDxfId="5"/>
+    <tableColumn id="2" name="BUG" dataDxfId="4"/>
+    <tableColumn id="4" name="NOTE" dataDxfId="3"/>
+    <tableColumn id="5" name="DATE" dataDxfId="2"/>
+    <tableColumn id="3" name="PRIORITY" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:D33" totalsRowShown="0" headerRowDxfId="0" dataCellStyle="Calculation">
+  <autoFilter ref="A1:D33"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="SEZIONE" dataCellStyle="Calculation"/>
+    <tableColumn id="3" name="TO FIX" dataCellStyle="Calculation"/>
+    <tableColumn id="4" name="NOTE" dataCellStyle="Calculation"/>
+    <tableColumn id="5" name="DATE" dataCellStyle="Calculation"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1221,216 +1308,216 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>47</v>
+      <c r="A1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="21"/>
+        <v>46</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="26"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="29"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="24"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="24"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="29"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="24"/>
+        <v>51</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="29"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="24"/>
+        <v>52</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="29"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="27"/>
+        <v>53</v>
+      </c>
+      <c r="H7" s="30"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="32"/>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>57</v>
+        <v>75</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="11"/>
+      <c r="A11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="10"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="11"/>
+      <c r="A18" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="10"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1444,19 +1531,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="68.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="3" max="3" width="68.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -1467,478 +1554,355 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="1"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="2">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2">
         <v>41876</v>
       </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2">
-        <v>41876</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="D3" s="2">
+        <v>41922</v>
+      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2">
-        <v>41876</v>
-      </c>
+      <c r="C4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="2">
+        <v>41922</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="2">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="2">
         <v>41922</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>107</v>
-      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" s="2">
-        <v>41922</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2">
+        <v>41876</v>
+      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E7" s="2">
-        <v>41922</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="2">
-        <v>41922</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D7" s="2">
+        <v>41876</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2">
+        <v>41876</v>
+      </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" s="2">
-        <v>41922</v>
-      </c>
+      <c r="C9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2">
+        <v>41905</v>
+      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="2">
+        <v>41</v>
+      </c>
+      <c r="D10" s="2">
         <v>41922</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="2">
-        <v>41876</v>
-      </c>
+      <c r="C11" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="2">
+        <v>41922</v>
+      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="2">
+        <v>95</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="2">
+        <v>41922</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2">
+        <v>41905</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="2">
         <v>41876</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="2">
-        <v>41876</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="2">
-        <v>41876</v>
-      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="2">
+      <c r="C15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="2">
         <v>41876</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="7">
-        <v>41876</v>
-      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="2">
+        <v>41905</v>
+      </c>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2">
+        <v>41922</v>
+      </c>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="2">
-        <v>41905</v>
-      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="2">
-        <v>41876</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="2">
-        <v>41876</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="2">
-        <v>41922</v>
-      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="2">
-        <v>41922</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="2">
-        <v>41876</v>
-      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E24" s="2">
-        <v>41922</v>
-      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E25" s="2">
-        <v>41922</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="2">
-        <v>41876</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="2">
-        <v>41876</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="2">
-        <v>41905</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="2">
-        <v>41876</v>
-      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="2">
-        <v>41876</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" s="2">
-        <v>41876</v>
-      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E32" s="2">
-        <v>41905</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E33" s="2">
-        <v>41922</v>
-      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1950,6 +1914,337 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="107" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="18"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="18"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="18"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+    </row>
+    <row r="21" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1966,50 +2261,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>41915</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="18">
+        <v>90</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="17">
         <v>41919</v>
       </c>
     </row>
@@ -2019,7 +2314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2034,19 +2329,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>87</v>
       </c>
+      <c r="B1" s="16" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>91</v>
+      <c r="A2" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
funzione changeState del booking aggiornata
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="109">
   <si>
     <t>SEZIONE</t>
   </si>
@@ -42,9 +42,6 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>TO FIX</t>
-  </si>
-  <si>
     <t>MODAL: lo scroll non funziona, scrolla la pagina sotto invece di quella sopra</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
   </si>
   <si>
     <t>booking - freight plan</t>
-  </si>
-  <si>
-    <t>DESCRIZIONE VOYAGE SELEZIONATI: nel caso di più di un voyage FROM:origin TO:transhipment FROM transhipment TO: destination</t>
   </si>
   <si>
     <t>documenti</t>
@@ -542,9 +536,6 @@
     <t>divisione delle charge in tipo revenues(visibili da agency /shipowner e modificabili da agency) e dei costs(visibili e modificabili da shipowner)</t>
   </si>
   <si>
-    <t>pulsanti che ciclano ad ogni azione</t>
-  </si>
-  <si>
     <t>files</t>
   </si>
   <si>
@@ -554,9 +545,6 @@
     <t>search booking</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>se torno su search non vengono resettati i valori (rimane book ref)</t>
   </si>
   <si>
@@ -591,13 +579,25 @@
   </si>
   <si>
     <t>PRIORITY</t>
+  </si>
+  <si>
+    <t>https://github.com/stefanpenner/ember-cli/issues/74</t>
+  </si>
+  <si>
+    <t>getting 404 not found error when refreshing web app deployed using ember cli</t>
+  </si>
+  <si>
+    <t>authorize/share</t>
+  </si>
+  <si>
+    <t>AUTHORIZE: autorizzo a vedere il booking con i tuoi permessi; SHARE: autorizzo a vedere il booking con i permessi di chi ha fatto lo share. PER GLI STATI EDIT E LOCK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -671,8 +671,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -706,6 +721,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -822,11 +849,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -871,6 +899,9 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -898,9 +929,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -1018,11 +1053,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:D33" totalsRowShown="0" headerRowDxfId="0" dataCellStyle="Calculation">
-  <autoFilter ref="A1:D33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:D32" totalsRowShown="0" headerRowDxfId="0" dataCellStyle="Calculation">
+  <autoFilter ref="A1:D32"/>
   <tableColumns count="4">
     <tableColumn id="1" name="SEZIONE" dataCellStyle="Calculation"/>
-    <tableColumn id="3" name="TO FIX" dataCellStyle="Calculation"/>
+    <tableColumn id="3" name="PRIORITY" dataCellStyle="Calculation"/>
     <tableColumn id="4" name="NOTE" dataCellStyle="Calculation"/>
     <tableColumn id="5" name="DATE" dataCellStyle="Calculation"/>
   </tableColumns>
@@ -1309,215 +1344,215 @@
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="26"/>
+        <v>44</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="27"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="29"/>
+        <v>45</v>
+      </c>
+      <c r="H3" s="28"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="30"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="29"/>
+        <v>48</v>
+      </c>
+      <c r="H4" s="28"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="30"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="29"/>
+        <v>49</v>
+      </c>
+      <c r="H5" s="28"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="30"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="29"/>
+        <v>50</v>
+      </c>
+      <c r="H6" s="28"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="30"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="32"/>
+        <v>51</v>
+      </c>
+      <c r="H7" s="31"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="33"/>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" s="10"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" s="10"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1560,16 +1595,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2">
         <v>41876</v>
@@ -1578,13 +1613,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D3" s="2">
         <v>41922</v>
@@ -1593,13 +1628,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D4" s="2">
         <v>41922</v>
@@ -1608,13 +1643,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D5" s="2">
         <v>41922</v>
@@ -1624,10 +1659,10 @@
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2">
         <v>41876</v>
@@ -1636,13 +1671,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D7" s="2">
         <v>41876</v>
@@ -1651,13 +1686,13 @@
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="D8" s="2">
         <v>41876</v>
@@ -1666,13 +1701,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2">
         <v>41905</v>
@@ -1681,13 +1716,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D10" s="2">
         <v>41922</v>
@@ -1696,13 +1731,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D11" s="2">
         <v>41922</v>
@@ -1711,13 +1746,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D12" s="2">
         <v>41922</v>
@@ -1726,13 +1761,13 @@
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2">
         <v>41905</v>
@@ -1741,13 +1776,13 @@
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D14" s="2">
         <v>41876</v>
@@ -1756,13 +1791,13 @@
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="2">
         <v>41876</v>
@@ -1771,13 +1806,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" s="2">
         <v>41905</v>
@@ -1786,13 +1821,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17" s="2">
         <v>41922</v>
@@ -1915,16 +1950,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="107" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
   </cols>
@@ -1934,7 +1969,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
@@ -1945,181 +1980,157 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>7</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B2" s="35"/>
       <c r="C2" s="21" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D2" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20" t="s">
-        <v>7</v>
-      </c>
+      <c r="B3" s="35"/>
       <c r="C3" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>107</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>96</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B4" s="34"/>
       <c r="C4" s="21" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
-      <c r="B5" s="20" t="s">
-        <v>7</v>
-      </c>
+      <c r="B5" s="34"/>
       <c r="C5" s="21" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>7</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B6" s="34"/>
       <c r="C6" s="21" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>7</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B7" s="36"/>
       <c r="C7" s="21" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="36"/>
+      <c r="C8" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="B12" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>107</v>
+      <c r="D12" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>107</v>
-      </c>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
@@ -2136,7 +2147,7 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="18"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2151,13 +2162,13 @@
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
     </row>
-    <row r="21" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
@@ -2228,12 +2239,6 @@
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2262,16 +2267,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>84</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>3</v>
@@ -2279,16 +2284,16 @@
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>81</v>
-      </c>
       <c r="D2" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E2" s="14">
         <v>41915</v>
@@ -2296,13 +2301,13 @@
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="B3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="E3" s="17">
         <v>41919</v>
@@ -2316,10 +2321,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2330,22 +2335,33 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>88</v>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="http://stackoverflow.com/questions/26129917/getting-404-not-found-error-when-refreshing-web-app-deployed-using-ember-cli"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sistemata funzione custom changestate
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="109">
   <si>
     <t>SEZIONE</t>
   </si>
@@ -902,6 +902,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -929,9 +932,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1357,18 +1357,18 @@
       <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="27"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="30"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1377,16 +1377,16 @@
       <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="30"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="33"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1395,16 +1395,16 @@
       <c r="B4" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="30"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="33"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1413,16 +1413,16 @@
       <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="30"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="33"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1431,16 +1431,16 @@
       <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="28"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="30"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="33"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1449,16 +1449,16 @@
       <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="31"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="33"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="36"/>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1953,7 +1953,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1982,7 +1982,7 @@
       <c r="A2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="35"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="21" t="s">
         <v>9</v>
       </c>
@@ -1991,20 +1991,24 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="20"/>
+      <c r="D3" s="22" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="21" t="s">
         <v>14</v>
       </c>
@@ -2014,7 +2018,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
-      <c r="B5" s="34"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="21" t="s">
         <v>15</v>
       </c>
@@ -2026,7 +2030,7 @@
       <c r="A6" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="21" t="s">
         <v>102</v>
       </c>
@@ -2038,7 +2042,7 @@
       <c r="A7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="36"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="21" t="s">
         <v>22</v>
       </c>
@@ -2050,7 +2054,7 @@
       <c r="A8" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="36"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="21" t="s">
         <v>96</v>
       </c>
@@ -2062,7 +2066,7 @@
       <c r="A9" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="36"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="21" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
risolto bug per unlock
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -14,8 +14,8 @@
   <sheets>
     <sheet name="GITHUB" sheetId="3" r:id="rId1"/>
     <sheet name="BUG - Seaoracle" sheetId="1" r:id="rId2"/>
-    <sheet name="TO-FIX Seaoracle" sheetId="6" r:id="rId3"/>
-    <sheet name="CHANGELOG - CLI-Sea" sheetId="2" r:id="rId4"/>
+    <sheet name="TO-FIX - Seaoracle" sheetId="6" r:id="rId3"/>
+    <sheet name="CHANGELOG - Seaoracle" sheetId="2" r:id="rId4"/>
     <sheet name="ERROR" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -1953,7 +1953,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2258,7 +2258,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
corretto errore upload exel
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="111">
   <si>
     <t>SEZIONE</t>
   </si>
@@ -592,12 +592,18 @@
   <si>
     <t>AUTHORIZE: autorizzo a vedere il booking con i tuoi permessi; SHARE: autorizzo a vedere il booking con i permessi di chi ha fatto lo share. PER GLI STATI EDIT E LOCK</t>
   </si>
+  <si>
+    <t>DTD</t>
+  </si>
+  <si>
+    <t>prepopolarla con la data di quando viene fatto il booking</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -686,8 +692,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -732,6 +745,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -854,7 +873,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -903,8 +922,22 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -932,13 +965,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="7">
     <dxf>
       <font>
         <strike val="0"/>
@@ -955,14 +989,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1039,14 +1065,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E32" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:E32"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="SEZIONE" dataDxfId="5"/>
-    <tableColumn id="2" name="BUG" dataDxfId="4"/>
-    <tableColumn id="4" name="NOTE" dataDxfId="3"/>
-    <tableColumn id="5" name="DATE" dataDxfId="2"/>
-    <tableColumn id="3" name="PRIORITY" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D31" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:D31"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="SEZIONE" dataDxfId="4"/>
+    <tableColumn id="2" name="BUG" dataDxfId="3"/>
+    <tableColumn id="4" name="NOTE" dataDxfId="2"/>
+    <tableColumn id="5" name="DATE" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1357,18 +1382,18 @@
       <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="30"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="42"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1377,16 +1402,16 @@
       <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="31"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="33"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="45"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1395,16 +1420,16 @@
       <c r="B4" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="31"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="33"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="45"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1413,16 +1438,16 @@
       <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="33"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="45"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1431,16 +1456,16 @@
       <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="31"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="33"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="45"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1449,16 +1474,16 @@
       <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="34"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="36"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="48"/>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1566,10 +1591,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1578,10 +1603,9 @@
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="68.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1594,350 +1618,310 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="29">
+        <v>41876</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="29">
+        <v>41905</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="37">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="29">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="37">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="37">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="37">
+        <v>41876</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
+      <c r="B9" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="37">
+        <v>41876</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="37">
+        <v>41876</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="37">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="37">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="37">
+        <v>41905</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="37">
+        <v>41876</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="37">
+        <v>41905</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="37">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D17" s="37">
         <v>41876</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="2">
-        <v>41922</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="2">
-        <v>41922</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="2">
-        <v>41922</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>41876</v>
-      </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="2">
-        <v>41876</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2">
-        <v>41876</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="2">
-        <v>41905</v>
-      </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="2">
-        <v>41922</v>
-      </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" s="2">
-        <v>41922</v>
-      </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="2">
-        <v>41922</v>
-      </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="2">
-        <v>41905</v>
-      </c>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="2">
-        <v>41876</v>
-      </c>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="2">
-        <v>41876</v>
-      </c>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="2">
-        <v>41905</v>
-      </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="2">
-        <v>41922</v>
-      </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="3"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="3"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1953,7 +1937,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,14 +1963,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="22" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2005,24 +1991,28 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="21" t="s">
+      <c r="B4" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="22" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="21" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="22" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2042,7 +2032,7 @@
       <c r="A7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="21" t="s">
         <v>22</v>
       </c>
@@ -2054,7 +2044,7 @@
       <c r="A8" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="27"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="21" t="s">
         <v>96</v>
       </c>
@@ -2066,7 +2056,7 @@
       <c r="A9" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="27"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="21" t="s">
         <v>27</v>
       </c>
@@ -2131,10 +2121,16 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="18"/>
+      <c r="A14" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>

</xml_diff>

<commit_message>
relase staile da testare
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23385" windowHeight="10605" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23385" windowHeight="10605" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GITHUB" sheetId="3" r:id="rId1"/>
@@ -873,7 +873,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -931,13 +931,13 @@
     <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -965,7 +965,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1593,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,10 +1619,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="39" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -1634,10 +1633,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="39" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1651,18 +1650,18 @@
       <c r="A4" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="29">
         <v>41922</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="38" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="30" t="s">
@@ -1679,18 +1678,18 @@
       <c r="A6" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="29">
         <v>41922</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="37" t="s">
         <v>100</v>
       </c>
       <c r="B7" s="34" t="s">
@@ -1699,38 +1698,38 @@
       <c r="C7" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="36">
         <v>41922</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="37" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="36">
         <v>41876</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="36">
         <v>41876</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="37" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="32" t="s">
@@ -1739,68 +1738,68 @@
       <c r="C10" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="36">
         <v>41876</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="37" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="36">
         <v>41922</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="37" t="s">
         <v>92</v>
       </c>
       <c r="B12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="37">
+      <c r="D12" s="36">
         <v>41922</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="37" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="37">
+      <c r="D13" s="36">
         <v>41905</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="37" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="36">
         <v>41876</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="37" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="31" t="s">
@@ -1809,12 +1808,12 @@
       <c r="C15" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="37">
+      <c r="D15" s="36">
         <v>41905</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="37" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="31" t="s">
@@ -1823,19 +1822,19 @@
       <c r="C16" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="37">
+      <c r="D16" s="36">
         <v>41922</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="31" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="37">
+      <c r="D17" s="36">
         <v>41876</v>
       </c>
     </row>
@@ -1936,7 +1935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
risolto bug newCode in new equipment
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="125">
   <si>
     <t>SEZIONE</t>
   </si>
@@ -598,12 +598,54 @@
   <si>
     <t>prepopolarla con la data di quando viene fatto il booking</t>
   </si>
+  <si>
+    <t>SIGN- UP</t>
+  </si>
+  <si>
+    <t>una volta eseguita l'azione i campi devono essere sbiancati e bisogna tornare sul login.</t>
+  </si>
+  <si>
+    <t>LOGO</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>è possibile caricare più di un logo… bisogna predisporre un controllo/warning?</t>
+  </si>
+  <si>
+    <t>FILES</t>
+  </si>
+  <si>
+    <t>se carico un file poi la scritta - MAX 10 MB - sparisce</t>
+  </si>
+  <si>
+    <t>NEW STAMP</t>
+  </si>
+  <si>
+    <t>il pulsante alla post continua a ciclare</t>
+  </si>
+  <si>
+    <t>AUTOCOMPLETE</t>
+  </si>
+  <si>
+    <t>Uncaught Error: Assertion Failed: calling set on destroyed object : quando premo con la freccia in giù… lo fa anche con input normali</t>
+  </si>
+  <si>
+    <t>se inserisco un equipment code che già esiste e poi ne inserisco un altro mi dice di verificare che il campo sia stato inserito</t>
+  </si>
+  <si>
+    <t>EQUIPMENT NEW</t>
+  </si>
+  <si>
+    <t>alla post non si cancellano campi current status e current status date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -699,8 +741,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -734,12 +791,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -873,7 +924,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -922,13 +973,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -937,7 +985,7 @@
     <xf numFmtId="14" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -965,6 +1013,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1064,8 +1126,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D31" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:D31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D30" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:D30"/>
   <tableColumns count="4">
     <tableColumn id="1" name="SEZIONE" dataDxfId="4"/>
     <tableColumn id="2" name="BUG" dataDxfId="3"/>
@@ -1381,18 +1443,18 @@
       <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="42"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="39"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1401,16 +1463,16 @@
       <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="45"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="42"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1419,16 +1481,16 @@
       <c r="B4" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="45"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="42"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1437,16 +1499,16 @@
       <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="45"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="42"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1455,16 +1517,16 @@
       <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="43"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="45"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="42"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1473,16 +1535,16 @@
       <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="46"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="48"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="45"/>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1590,10 +1652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,272 +1681,296 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="27">
         <v>41876</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="27">
         <v>41905</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="27">
         <v>41922</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="27">
         <v>41922</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="27">
         <v>41922</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="33">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="33">
+        <v>41876</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="33">
+        <v>41876</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="33">
+        <v>41876</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="29"/>
+      <c r="C11" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="33">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="33">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="33">
+        <v>41905</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="33">
+        <v>41876</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="33">
+        <v>41905</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="33">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="46"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="49">
+        <v>41876</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="50"/>
+      <c r="C18" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="33">
+        <v>41928</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="52">
+        <v>41928</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="33">
+        <v>41928</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="31"/>
+      <c r="C21" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" s="33">
+        <v>41928</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="30"/>
+      <c r="C22" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="33">
+        <v>41928</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="36">
-        <v>41922</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="36">
-        <v>41876</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="36">
-        <v>41876</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="36">
-        <v>41876</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" s="36">
-        <v>41922</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="36">
-        <v>41922</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="36">
-        <v>41905</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="36">
-        <v>41876</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="36">
-        <v>41905</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="36">
-        <v>41922</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="36">
-        <v>41876</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="C23" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="27">
+        <v>41928</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="2"/>
+      <c r="A24" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="33">
+        <v>41928</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="2"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -1893,16 +1979,16 @@
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="5"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
+      <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="2"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
@@ -1915,12 +2001,6 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1936,7 +2016,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1965,7 +2045,7 @@
       <c r="A2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="36" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="23" t="s">
@@ -1993,7 +2073,7 @@
       <c r="A4" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="36" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="23" t="s">
@@ -2005,7 +2085,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="36" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="23" t="s">
@@ -2120,14 +2200,16 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="21" t="s">
+      <c r="B14" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="22" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>

<commit_message>
route application con #
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="129">
   <si>
     <t>SEZIONE</t>
   </si>
@@ -639,6 +639,18 @@
   </si>
   <si>
     <t>alla post non si cancellano campi current status e current status date</t>
+  </si>
+  <si>
+    <t>VOYAGE - DETAILS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">se inserisco un estimated arrival non viene automaticamente compilato il departure </t>
+  </si>
+  <si>
+    <t>ERROR MANCANZA LOGO</t>
+  </si>
+  <si>
+    <t>và gestito mostrando all'utente</t>
   </si>
 </sst>
 </file>
@@ -924,13 +936,10 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -986,6 +995,20 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1013,20 +1036,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1429,10 +1438,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1443,18 +1452,18 @@
       <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="39"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="48"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1463,34 +1472,34 @@
       <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="42"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="51"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B4" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="40"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="42"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="51"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1499,16 +1508,16 @@
       <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="40"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="42"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="51"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1517,16 +1526,16 @@
       <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="40"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="42"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="51"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1535,22 +1544,22 @@
       <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="43"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="44"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="45"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="54"/>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1571,10 +1580,10 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="9"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1613,10 +1622,10 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="10"/>
+      <c r="B18" s="9"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1654,8 +1663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,321 +1676,333 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="26">
         <v>41876</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="26">
         <v>41905</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="26">
         <v>41922</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="26">
         <v>41922</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="26">
         <v>41922</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="30" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="32">
         <v>41922</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="32" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="32">
         <v>41876</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="32" t="s">
+      <c r="A9" s="33"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="32">
         <v>41876</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="32">
         <v>41876</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="32" t="s">
+      <c r="B11" s="28"/>
+      <c r="C11" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="32">
         <v>41922</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="32" t="s">
+      <c r="B12" s="28"/>
+      <c r="C12" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="32">
         <v>41922</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="32" t="s">
+      <c r="B13" s="27"/>
+      <c r="C13" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="32">
         <v>41905</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="32" t="s">
+      <c r="B14" s="27"/>
+      <c r="C14" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D14" s="32">
         <v>41876</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="30" t="s">
+      <c r="B15" s="27"/>
+      <c r="C15" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="32">
         <v>41905</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="30" t="s">
+      <c r="B16" s="27"/>
+      <c r="C16" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="32">
         <v>41922</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="46"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="48" t="s">
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="49">
+      <c r="D17" s="39">
         <v>41876</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="54" t="s">
+      <c r="B18" s="40"/>
+      <c r="C18" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="32">
         <v>41928</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="D19" s="52">
+      <c r="D19" s="42">
         <v>41928</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="30" t="s">
+      <c r="B20" s="28"/>
+      <c r="C20" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20" s="32">
         <v>41928</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="30" t="s">
+      <c r="B21" s="30"/>
+      <c r="C21" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="32">
         <v>41928</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="32" t="s">
+      <c r="B22" s="28"/>
+      <c r="C22" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="32">
         <v>41928</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="26">
         <v>41928</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="28"/>
+      <c r="C24" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="33">
+      <c r="D24" s="32">
         <v>41928</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="30"/>
+      <c r="C25" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" s="32">
+        <v>41928</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="A26" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="30"/>
+      <c r="C26" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="32">
+        <v>41928</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
+      <c r="A27" s="4"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="5"/>
+      <c r="C27" s="44"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2028,298 +2049,298 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="36" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="21" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="21" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="21" t="s">
+      <c r="B9" s="25"/>
+      <c r="C9" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="21" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="21" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="18"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="17"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="18"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="17"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
     </row>
     <row r="20" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2347,36 +2368,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="13">
         <v>41915</v>
       </c>
     </row>
@@ -2387,10 +2408,10 @@
       <c r="B3" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <v>41919</v>
       </c>
     </row>
@@ -2415,23 +2436,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>106</v>
       </c>
       <c r="B3" t="s">

</xml_diff>

<commit_message>
versione da testare aggiornata ember-cli
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="135">
   <si>
     <t>SEZIONE</t>
   </si>
@@ -663,6 +663,12 @@
   </si>
   <si>
     <t>senza voyage non produce nulla</t>
+  </si>
+  <si>
+    <t>DELETE BOOKING</t>
+  </si>
+  <si>
+    <t>agginugere pulsanti per la rimozione per l'AGENZIA</t>
   </si>
 </sst>
 </file>
@@ -948,10 +954,9 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1450,10 +1455,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1464,18 +1469,18 @@
       <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="48"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="47"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1484,34 +1489,34 @@
       <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="49"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="51"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="50"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B4" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="49"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="51"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="50"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1520,16 +1525,16 @@
       <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="51"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="50"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1538,16 +1543,16 @@
       <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="49"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="50"/>
-      <c r="P6" s="50"/>
-      <c r="Q6" s="51"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="50"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1556,22 +1561,22 @@
       <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="54"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="53"/>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1592,10 +1597,10 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="9"/>
+      <c r="B11" s="8"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1634,10 +1639,10 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="9"/>
+      <c r="B18" s="8"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1675,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,272 +1693,272 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="25">
         <v>41876</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="25">
         <v>41905</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="25">
         <v>41922</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>41922</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="25">
         <v>41922</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="29" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="31">
         <v>41922</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="31" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="31">
         <v>41876</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="31" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <v>41876</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29" t="s">
+      <c r="B10" s="27"/>
+      <c r="C10" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="31">
         <v>41876</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="31" t="s">
+      <c r="B11" s="27"/>
+      <c r="C11" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="31">
         <v>41922</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="31" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="31">
         <v>41922</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="31" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="31">
         <v>41905</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="31" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="31">
         <v>41876</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="29" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="31">
         <v>41905</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="29" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="31">
         <v>41922</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="29" t="s">
+      <c r="B17" s="29"/>
+      <c r="C17" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="D17" s="32"/>
+      <c r="D17" s="31"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="29" t="s">
+      <c r="B18" s="27"/>
+      <c r="C18" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="32"/>
+      <c r="D18" s="31"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="38" t="s">
+      <c r="A19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="39">
+      <c r="D19" s="38">
         <v>41876</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="44" t="s">
+      <c r="B20" s="39"/>
+      <c r="C20" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="31">
         <v>41928</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="41">
         <v>41928</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29" t="s">
+      <c r="B22" s="27"/>
+      <c r="C22" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="31">
         <v>41928</v>
       </c>
     </row>
@@ -1961,81 +1966,91 @@
       <c r="A23" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="29" t="s">
+      <c r="B23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="25">
         <v>41928</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="31" t="s">
+      <c r="B24" s="27"/>
+      <c r="C24" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="31">
         <v>41928</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="25">
         <v>41928</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="44" t="s">
+      <c r="B26" s="27"/>
+      <c r="C26" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="31">
         <v>41928</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="44" t="s">
+      <c r="B27" s="29"/>
+      <c r="C27" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="31">
         <v>41928</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="44" t="s">
+      <c r="B28" s="29"/>
+      <c r="C28" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="31">
         <v>41928</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="2"/>
+      <c r="A29" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="25">
+        <v>41932</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
@@ -2081,298 +2096,298 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="35" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="20" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="20" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="20" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="20" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="20" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="17"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="17"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="16"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2400,36 +2415,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <v>41915</v>
       </c>
     </row>
@@ -2440,10 +2455,10 @@
       <c r="B3" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="15">
         <v>41919</v>
       </c>
     </row>
@@ -2468,23 +2483,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>106</v>
       </c>
       <c r="B3" t="s">

</xml_diff>

<commit_message>
eliminato errore localstorage grants
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="138">
   <si>
     <t>SEZIONE</t>
   </si>
@@ -608,12 +608,6 @@
     <t>LOGO</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>è possibile caricare più di un logo… bisogna predisporre un controllo/warning?</t>
-  </si>
-  <si>
     <t>FILES</t>
   </si>
   <si>
@@ -669,6 +663,21 @@
   </si>
   <si>
     <t>agginugere pulsanti per la rimozione per l'AGENZIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">è possibile caricare più di un logo… rimuovere precedente logo </t>
+  </si>
+  <si>
+    <t>errore non rilevato</t>
+  </si>
+  <si>
+    <t>gestito lato server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEARCH  </t>
+  </si>
+  <si>
+    <t>aggiunta del campo 'no results'</t>
   </si>
 </sst>
 </file>
@@ -954,7 +963,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1017,7 +1026,6 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1052,6 +1060,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1469,18 +1483,18 @@
       <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="47"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="46"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1489,16 +1503,16 @@
       <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="48"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="50"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="49"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1507,16 +1521,16 @@
       <c r="B4" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="50"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="49"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1525,16 +1539,16 @@
       <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="48"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="50"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="49"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1543,16 +1557,16 @@
       <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="48"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="49"/>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="50"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="49"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1561,16 +1575,16 @@
       <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="51"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="53"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="52"/>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1681,7 +1695,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1895,22 +1909,26 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" s="31"/>
+      <c r="A17" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" s="25">
+        <v>41932</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B18" s="27"/>
       <c r="C18" s="28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D18" s="31"/>
     </row>
@@ -1929,7 +1947,7 @@
         <v>111</v>
       </c>
       <c r="B20" s="39"/>
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="42" t="s">
         <v>112</v>
       </c>
       <c r="D20" s="31">
@@ -1937,26 +1955,26 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="C21" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="D21" s="41">
+      <c r="B21" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" s="25">
         <v>41928</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D22" s="31">
         <v>41928</v>
@@ -1964,13 +1982,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D23" s="25">
         <v>41928</v>
@@ -1978,11 +1996,11 @@
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D24" s="31">
         <v>41928</v>
@@ -1990,13 +2008,13 @@
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D25" s="25">
         <v>41928</v>
@@ -2004,11 +2022,11 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B26" s="27"/>
-      <c r="C26" s="43" t="s">
-        <v>124</v>
+      <c r="C26" s="42" t="s">
+        <v>122</v>
       </c>
       <c r="D26" s="31">
         <v>41928</v>
@@ -2016,47 +2034,55 @@
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B27" s="29"/>
-      <c r="C27" s="43" t="s">
-        <v>126</v>
+      <c r="C27" s="42" t="s">
+        <v>124</v>
       </c>
       <c r="D27" s="31">
         <v>41928</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="D28" s="31">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="54" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="40">
         <v>41928</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D29" s="25">
         <v>41932</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="A30" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="29"/>
+      <c r="C30" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" s="31">
+        <v>41932</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>

</xml_diff>

<commit_message>
inserita ricerca con loading
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23385" windowHeight="10605" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23385" windowHeight="10605" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GITHUB" sheetId="3" r:id="rId1"/>
@@ -845,7 +845,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -957,13 +957,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -993,9 +1030,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1034,6 +1068,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1061,10 +1101,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="6" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1483,18 +1532,18 @@
       <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="47"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1503,16 +1552,16 @@
       <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="47"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="49"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="50"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1521,16 +1570,16 @@
       <c r="B4" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="49"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="50"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1539,16 +1588,16 @@
       <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="47"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="49"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="50"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1557,16 +1606,16 @@
       <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="47"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="49"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="50"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1575,16 +1624,16 @@
       <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="50"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="51"/>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="52"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="53"/>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1694,8 +1743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,7 +1770,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1730,12 +1779,12 @@
       <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="24">
         <v>41876</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1744,12 +1793,12 @@
       <c r="C3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="24">
         <v>41905</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="32" t="s">
         <v>90</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1758,12 +1807,12 @@
       <c r="C4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="24">
         <v>41922</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="32" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1772,12 +1821,12 @@
       <c r="C5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <v>41922</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="32" t="s">
         <v>97</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1786,130 +1835,130 @@
       <c r="C6" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="24">
         <v>41922</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="28" t="s">
+      <c r="B7" s="28"/>
+      <c r="C7" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="30">
         <v>41922</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="30" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="30">
         <v>41876</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="30" t="s">
+      <c r="A9" s="31"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="30">
         <v>41876</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="30">
         <v>41876</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="30" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="30">
         <v>41922</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="30" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="30">
         <v>41922</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="30" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="30">
         <v>41905</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="30" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="30">
         <v>41876</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="28" t="s">
+      <c r="B15" s="25"/>
+      <c r="C15" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="30">
         <v>41905</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="28" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="30">
         <v>41922</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="32" t="s">
         <v>129</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1918,70 +1967,70 @@
       <c r="C17" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="24">
         <v>41932</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28" t="s">
+      <c r="B18" s="26"/>
+      <c r="C18" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="31"/>
+      <c r="D18" s="30"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="37" t="s">
+      <c r="A19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="37">
         <v>41876</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="42" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="30">
         <v>41928</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="32" t="s">
         <v>113</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="24">
         <v>41928</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28" t="s">
+      <c r="B22" s="26"/>
+      <c r="C22" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="30">
         <v>41928</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="32" t="s">
         <v>116</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1990,24 +2039,24 @@
       <c r="C23" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="24">
         <v>41928</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="30" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="30">
         <v>41928</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="32" t="s">
         <v>121</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -2016,50 +2065,50 @@
       <c r="C25" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="24">
         <v>41928</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="42" t="s">
+      <c r="B26" s="26"/>
+      <c r="C26" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="D26" s="31">
+      <c r="D26" s="30">
         <v>41928</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="42" t="s">
+      <c r="B27" s="28"/>
+      <c r="C27" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="D27" s="31">
+      <c r="D27" s="30">
         <v>41928</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="C28" s="54" t="s">
+      <c r="C28" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="D28" s="40">
+      <c r="D28" s="39">
         <v>41928</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="32" t="s">
         <v>131</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2068,19 +2117,7 @@
       <c r="C29" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D29" s="25">
-        <v>41932</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
-        <v>136</v>
-      </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="D30" s="31">
+      <c r="D29" s="24">
         <v>41932</v>
       </c>
     </row>
@@ -2109,8 +2146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,188 +2173,194 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="34" t="s">
+      <c r="A5" s="19"/>
+      <c r="B5" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="19" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="17" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="19" t="s">
+      <c r="B8" s="23"/>
+      <c r="C8" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="17" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="56" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="54" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="16"/>
+      <c r="A15" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" s="59">
+        <v>41932</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="16"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="57"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
@@ -2525,7 +2568,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>106</v>
       </c>
       <c r="B3" t="s">

</xml_diff>

<commit_message>
versione 21-10 da testare
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23385" windowHeight="10605" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23385" windowHeight="10605" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GITHUB" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="136">
   <si>
     <t>SEZIONE</t>
   </si>
@@ -61,12 +61,6 @@
   </si>
   <si>
     <t>Save record</t>
-  </si>
-  <si>
-    <t>Voyage</t>
-  </si>
-  <si>
-    <t>NEW VOY: se ne creo uno nuovo ho la possibilità di salvarlo con un NUMBER vuoto</t>
   </si>
   <si>
     <t>Equipment</t>
@@ -1000,7 +994,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1041,7 +1035,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1055,11 +1048,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1073,33 +1061,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1110,12 +1071,48 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="6" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="6" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1519,215 +1516,215 @@
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="47"/>
+        <v>42</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="46"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="48"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="50"/>
+        <v>43</v>
+      </c>
+      <c r="H3" s="47"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="49"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="50"/>
+        <v>46</v>
+      </c>
+      <c r="H4" s="47"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="49"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="48"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="50"/>
+        <v>47</v>
+      </c>
+      <c r="H5" s="47"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="49"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="48"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="49"/>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="50"/>
+        <v>48</v>
+      </c>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="49"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" s="51"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="53"/>
+        <v>49</v>
+      </c>
+      <c r="H7" s="50"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="52"/>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" s="8"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B18" s="8"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1743,8 +1740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,357 +1766,357 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="24">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="29">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="29">
         <v>41876</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="24">
-        <v>41905</v>
-      </c>
-    </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="29">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D5" s="29">
         <v>41922</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="24">
-        <v>41922</v>
-      </c>
-    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" s="24">
-        <v>41922</v>
-      </c>
+      <c r="A6" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="30">
+        <v>31</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="23">
+        <v>41905</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="23">
         <v>41922</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="30">
-        <v>41876</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="30">
-        <v>41876</v>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="23">
+        <v>41922</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="30">
+        <v>95</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="23">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="29">
         <v>41876</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" s="30">
-        <v>41922</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="30">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="23">
+        <v>41876</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="56"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="59">
+        <v>41876</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="29">
+        <v>41905</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="29">
+        <v>41876</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="29">
+        <v>41905</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="29">
         <v>41922</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="30">
-        <v>41905</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="30">
-        <v>41876</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="30">
-        <v>41905</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="30">
-        <v>41922</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="B17" s="3" t="s">
+    <row r="18" spans="1:4" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" s="24">
+      <c r="C18" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="63">
         <v>41932</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="D18" s="30"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="34"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="37">
-        <v>41876</v>
+    <row r="19" spans="1:4" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="29">
+        <v>41928</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="41" t="s">
+      <c r="A20" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="29">
+        <v>41928</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="30">
+      <c r="B21" s="26"/>
+      <c r="C21" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="29">
         <v>41928</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C21" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="D21" s="24">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="29">
         <v>41928</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22" s="30">
-        <v>41928</v>
-      </c>
-    </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" s="24">
+      <c r="A23" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="29">
         <v>41928</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="D24" s="30">
+        <v>111</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="D24" s="23">
         <v>41928</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
-        <v>121</v>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>114</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25" s="24">
+      <c r="C25" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="23">
         <v>41928</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="D26" s="30">
+        <v>119</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="23">
         <v>41928</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="41" t="s">
+      <c r="B27" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="D27" s="30">
+      <c r="D27" s="33">
         <v>41928</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="B28" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="C28" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="D28" s="39">
-        <v>41928</v>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" s="23">
+        <v>41932</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D29" s="24">
-        <v>41932</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
@@ -2146,8 +2143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2163,7 +2160,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -2176,130 +2173,132 @@
       <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="32" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>101</v>
-      </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="23"/>
+        <v>19</v>
+      </c>
+      <c r="B7" s="22"/>
       <c r="C7" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="23"/>
+        <v>93</v>
+      </c>
+      <c r="B8" s="22"/>
       <c r="C8" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="B9" s="22"/>
       <c r="C9" s="18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -2313,54 +2312,56 @@
         <v>8</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" s="55" t="s">
+      <c r="A14" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="56" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="54" t="s">
-        <v>103</v>
+      <c r="C14" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="60" t="s">
-        <v>137</v>
-      </c>
-      <c r="D15" s="59">
+      <c r="A15" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" s="54">
         <v>41932</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="57"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="57"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="42"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
@@ -2485,16 +2486,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>3</v>
@@ -2502,16 +2503,16 @@
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>79</v>
-      </c>
       <c r="D2" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E2" s="12">
         <v>41915</v>
@@ -2519,13 +2520,13 @@
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="B3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="E3" s="15">
         <v>41919</v>
@@ -2553,26 +2554,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sistemazione dashboard 22 ottobre
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="140">
   <si>
     <t>SEZIONE</t>
   </si>
@@ -672,6 +672,18 @@
   </si>
   <si>
     <t>se scendo nel menù a tendina con KeyDown lo scroll non segue il movimento</t>
+  </si>
+  <si>
+    <t>http://gevious.github.io/ember-datepicker/</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>DASHBOARD</t>
+  </si>
+  <si>
+    <t>pulsanti con colori grigi in test</t>
   </si>
 </sst>
 </file>
@@ -994,7 +1006,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1076,13 +1088,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1110,14 +1120,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1210,20 +1231,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D32" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:D32"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="SEZIONE" dataDxfId="4"/>
-    <tableColumn id="2" name="BUG" dataDxfId="3"/>
-    <tableColumn id="4" name="NOTE" dataDxfId="2"/>
-    <tableColumn id="5" name="DATE" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E32" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:E32"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="SEZIONE" dataDxfId="5"/>
+    <tableColumn id="2" name="BUG" dataDxfId="4"/>
+    <tableColumn id="4" name="NOTE" dataDxfId="3"/>
+    <tableColumn id="3" name="Link" dataDxfId="0"/>
+    <tableColumn id="5" name="DATE" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:D32" totalsRowShown="0" headerRowDxfId="0" dataCellStyle="Calculation">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:D32" totalsRowShown="0" headerRowDxfId="1" dataCellStyle="Calculation">
   <autoFilter ref="A1:D32"/>
   <tableColumns count="4">
     <tableColumn id="1" name="SEZIONE" dataCellStyle="Calculation"/>
@@ -1527,18 +1549,18 @@
       <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="56"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1547,16 +1569,16 @@
       <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="57"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="59"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="57"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1565,16 +1587,16 @@
       <c r="B4" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="59"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="57"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1583,16 +1605,16 @@
       <c r="B5" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="57"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="59"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="57"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1601,16 +1623,16 @@
       <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="57"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="59"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="57"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1619,16 +1641,16 @@
       <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="60"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61"/>
-      <c r="M7" s="61"/>
-      <c r="N7" s="61"/>
-      <c r="O7" s="61"/>
-      <c r="P7" s="61"/>
-      <c r="Q7" s="62"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="60"/>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1736,21 +1758,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="68.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1761,10 +1784,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>98</v>
       </c>
@@ -1772,11 +1798,12 @@
       <c r="C2" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="26"/>
+      <c r="E2" s="29">
         <v>41922</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>26</v>
       </c>
@@ -1784,11 +1811,12 @@
       <c r="C3" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="28"/>
+      <c r="E3" s="29">
         <v>41876</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>23</v>
       </c>
@@ -1796,11 +1824,12 @@
       <c r="C4" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="28"/>
+      <c r="E4" s="29">
         <v>41922</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>90</v>
       </c>
@@ -1808,21 +1837,25 @@
       <c r="C5" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="28"/>
+      <c r="E5" s="29">
         <v>41922</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26" t="s">
+      <c r="B6" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="D6" s="29"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="63"/>
+      <c r="E6" s="33"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>31</v>
       </c>
@@ -1832,11 +1865,12 @@
       <c r="C7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="3"/>
+      <c r="E7" s="23">
         <v>41905</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>88</v>
       </c>
@@ -1846,11 +1880,12 @@
       <c r="C8" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="3"/>
+      <c r="E8" s="23">
         <v>41922</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>36</v>
       </c>
@@ -1860,11 +1895,12 @@
       <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="3"/>
+      <c r="E9" s="23">
         <v>41922</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>95</v>
       </c>
@@ -1874,21 +1910,23 @@
       <c r="C10" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="3"/>
+      <c r="E10" s="23">
         <v>41922</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="30"/>
       <c r="B11" s="24"/>
       <c r="C11" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="28"/>
+      <c r="E11" s="29">
         <v>41876</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>16</v>
       </c>
@@ -1898,57 +1936,70 @@
       <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="3"/>
+      <c r="E12" s="23">
         <v>41876</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="46"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48" t="s">
+      <c r="B13" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="49">
+      <c r="D13" s="61"/>
+      <c r="E13" s="62">
         <v>41876</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="28" t="s">
+      <c r="B14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="4"/>
+      <c r="E14" s="23">
         <v>41905</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="28" t="s">
+      <c r="B15" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="34"/>
+      <c r="E15" s="33">
         <v>41876</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="26" t="s">
+      <c r="B16" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="63"/>
+      <c r="E16" s="33">
         <v>41905</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>33</v>
       </c>
@@ -1956,39 +2007,44 @@
       <c r="C17" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" s="29">
         <v>41922</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="50" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51" t="s">
+    <row r="18" spans="1:5" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="D18" s="53">
+      <c r="D18" s="49"/>
+      <c r="E18" s="50">
         <v>41932</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="B19" s="63" t="s">
+      <c r="B19" s="51" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="36"/>
+      <c r="E19" s="23">
         <v>41928</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>109</v>
       </c>
@@ -1998,35 +2054,38 @@
       <c r="C20" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="36"/>
+      <c r="E20" s="23">
         <v>41928</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="B21" s="26"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="29">
+      <c r="D21" s="26"/>
+      <c r="E21" s="29">
         <v>41928</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="26"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="28"/>
+      <c r="E22" s="29">
         <v>41934</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>118</v>
       </c>
@@ -2036,11 +2095,12 @@
       <c r="C23" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="36"/>
+      <c r="E23" s="23">
         <v>41928</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>111</v>
       </c>
@@ -2050,11 +2110,12 @@
       <c r="C24" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="36"/>
+      <c r="E24" s="23">
         <v>41928</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>114</v>
       </c>
@@ -2064,11 +2125,12 @@
       <c r="C25" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="3"/>
+      <c r="E25" s="23">
         <v>41928</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>118</v>
       </c>
@@ -2078,11 +2140,12 @@
       <c r="C26" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="4"/>
+      <c r="E26" s="23">
         <v>41928</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
         <v>122</v>
       </c>
@@ -2092,11 +2155,12 @@
       <c r="C27" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="D27" s="33">
+      <c r="D27" s="37"/>
+      <c r="E27" s="33">
         <v>41928</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>128</v>
       </c>
@@ -2106,33 +2170,44 @@
       <c r="C28" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="4"/>
+      <c r="E28" s="23">
         <v>41932</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="64">
+        <v>41934</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
versione da testare 22 ott
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="141">
   <si>
     <t>SEZIONE</t>
   </si>
@@ -671,9 +671,6 @@
     <t>aggiunta del campo 'no results'</t>
   </si>
   <si>
-    <t>se scendo nel menù a tendina con KeyDown lo scroll non segue il movimento</t>
-  </si>
-  <si>
     <t>http://gevious.github.io/ember-datepicker/</t>
   </si>
   <si>
@@ -684,6 +681,15 @@
   </si>
   <si>
     <t>pulsanti con colori grigi in test</t>
+  </si>
+  <si>
+    <t>WARNING</t>
+  </si>
+  <si>
+    <t>1. Se scendo nel menù a tendina con KeyDown lo scroll non segue il movimento.
+2. Se focus-In deve aprirsi lista elementi.
+3. Togliere azione su lente di ingrandimento (si apre la lista).
+4. Se cerco di eliminare un elemento precedentemente selezionato l'azione non parte.</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1012,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1093,37 +1099,45 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1131,14 +1145,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1155,6 +1161,14 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1237,15 +1251,15 @@
     <tableColumn id="1" name="SEZIONE" dataDxfId="5"/>
     <tableColumn id="2" name="BUG" dataDxfId="4"/>
     <tableColumn id="4" name="NOTE" dataDxfId="3"/>
-    <tableColumn id="3" name="Link" dataDxfId="0"/>
-    <tableColumn id="5" name="DATE" dataDxfId="2"/>
+    <tableColumn id="3" name="Link" dataDxfId="2"/>
+    <tableColumn id="5" name="DATE" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:D32" totalsRowShown="0" headerRowDxfId="1" dataCellStyle="Calculation">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:D32" totalsRowShown="0" headerRowDxfId="0" dataCellStyle="Calculation">
   <autoFilter ref="A1:D32"/>
   <tableColumns count="4">
     <tableColumn id="1" name="SEZIONE" dataCellStyle="Calculation"/>
@@ -1549,18 +1563,18 @@
       <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="54"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1569,16 +1583,16 @@
       <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="57"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="63"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1587,16 +1601,16 @@
       <c r="B4" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="57"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="63"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1605,16 +1619,16 @@
       <c r="B5" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="55"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="56"/>
-      <c r="P5" s="56"/>
-      <c r="Q5" s="57"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="63"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1623,16 +1637,16 @@
       <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="55"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="57"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="62"/>
+      <c r="Q6" s="63"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1641,16 +1655,16 @@
       <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="60"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="66"/>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1760,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,7 +1783,7 @@
     <col min="1" max="1" width="29.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="62.140625" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1784,7 +1798,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -1803,16 +1817,16 @@
         <v>41922</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="25"/>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="56" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="28"/>
-      <c r="E3" s="29">
+      <c r="E3" s="57">
         <v>41876</v>
       </c>
     </row>
@@ -1830,15 +1844,17 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="28" t="s">
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29">
+      <c r="D5" s="4"/>
+      <c r="E5" s="23">
         <v>41922</v>
       </c>
     </row>
@@ -1849,10 +1865,10 @@
       <c r="B6" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="D6" s="63"/>
+      <c r="D6" s="54"/>
       <c r="E6" s="33"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1916,13 +1932,15 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="28" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="29">
+      <c r="D11" s="34"/>
+      <c r="E11" s="33">
         <v>41876</v>
       </c>
     </row>
@@ -1949,8 +1967,8 @@
       <c r="C13" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="61"/>
-      <c r="E13" s="62">
+      <c r="D13" s="52"/>
+      <c r="E13" s="53">
         <v>41876</v>
       </c>
     </row>
@@ -1991,10 +2009,10 @@
       <c r="B16" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="63" t="s">
+      <c r="C16" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="63"/>
+      <c r="D16" s="54"/>
       <c r="E16" s="33">
         <v>41905</v>
       </c>
@@ -2008,7 +2026,7 @@
         <v>34</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E17" s="29">
         <v>41922</v>
@@ -2072,20 +2090,20 @@
         <v>41928</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+    <row r="22" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="55" t="s">
         <v>116</v>
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="28" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D22" s="28"/>
       <c r="E22" s="29">
         <v>41934</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>118</v>
       </c>
@@ -2176,15 +2194,17 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="64">
+      <c r="D29" s="3"/>
+      <c r="E29" s="23">
         <v>41934</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fine fase di test 24/10/2014
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="145">
   <si>
     <t>SEZIONE</t>
   </si>
@@ -690,6 +690,18 @@
 2. Se focus-In deve aprirsi lista elementi.
 3. Togliere azione su lente di ingrandimento (si apre la lista).
 4. Se cerco di eliminare un elemento precedentemente selezionato l'azione non parte.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncaught TypeError: Cannot read property 'addClass' of undefined. Legato al 'no results' con addClass(hdn) </t>
+  </si>
+  <si>
+    <t>quando fa il loading se faccio scroll down compare loading more dell infinite scroll</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>confirm su goods non produce effetti (a volte và)</t>
   </si>
 </sst>
 </file>
@@ -857,7 +869,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -970,39 +982,113 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="0"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="0"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="0"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1012,7 +1098,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1041,19 +1127,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1065,7 +1141,6 @@
     <xf numFmtId="14" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1077,22 +1152,6 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="6" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1138,6 +1197,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1163,6 +1289,14 @@
           <bgColor theme="5"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1245,8 +1379,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E32" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:E32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E50" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:E50"/>
   <tableColumns count="5">
     <tableColumn id="1" name="SEZIONE" dataDxfId="5"/>
     <tableColumn id="2" name="BUG" dataDxfId="4"/>
@@ -1563,18 +1697,18 @@
       <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="H2" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="60"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="45"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1583,16 +1717,16 @@
       <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="63"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="48"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1601,16 +1735,16 @@
       <c r="B4" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="61"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
-      <c r="M4" s="62"/>
-      <c r="N4" s="62"/>
-      <c r="O4" s="62"/>
-      <c r="P4" s="62"/>
-      <c r="Q4" s="63"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="48"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1619,16 +1753,16 @@
       <c r="B5" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="63"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="48"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1637,16 +1771,16 @@
       <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
-      <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="63"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="48"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1655,16 +1789,16 @@
       <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="64"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65"/>
-      <c r="O7" s="65"/>
-      <c r="P7" s="65"/>
-      <c r="Q7" s="66"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="51"/>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1772,10 +1906,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,46 +1939,46 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="29">
+      <c r="D2" s="20"/>
+      <c r="E2" s="23">
         <v>41922</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="56" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="57">
+      <c r="D3" s="22"/>
+      <c r="E3" s="42">
         <v>41876</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="28" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29">
+      <c r="D4" s="22"/>
+      <c r="E4" s="23">
         <v>41922</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="25" t="s">
         <v>90</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1854,25 +1988,25 @@
         <v>91</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="23">
+      <c r="E5" s="17">
         <v>41922</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="33"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="26"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1882,12 +2016,12 @@
         <v>32</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="23">
+      <c r="E7" s="17">
         <v>41905</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="25" t="s">
         <v>88</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1897,12 +2031,12 @@
         <v>89</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="23">
+      <c r="E8" s="17">
         <v>41922</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="25" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1912,12 +2046,12 @@
         <v>37</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="23">
+      <c r="E9" s="17">
         <v>41922</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="25" t="s">
         <v>95</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1927,25 +2061,25 @@
         <v>96</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="23">
+      <c r="E10" s="17">
         <v>41922</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="33">
+      <c r="D11" s="27"/>
+      <c r="E11" s="26">
         <v>41876</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1955,25 +2089,25 @@
         <v>17</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="23">
+      <c r="E12" s="17">
         <v>41876</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="34" t="s">
+      <c r="A13" s="31"/>
+      <c r="B13" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="52"/>
-      <c r="E13" s="53">
+      <c r="D13" s="37"/>
+      <c r="E13" s="38">
         <v>41876</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="25" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1983,158 +2117,158 @@
         <v>30</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="23">
+      <c r="E14" s="17">
         <v>41905</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="33">
+      <c r="D15" s="27"/>
+      <c r="E15" s="26">
         <v>41876</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="54"/>
-      <c r="E16" s="33">
+      <c r="D16" s="39"/>
+      <c r="E16" s="26">
         <v>41905</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="26" t="s">
+      <c r="B17" s="18"/>
+      <c r="C17" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="23">
         <v>41922</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="48" t="s">
+    <row r="18" spans="1:5" s="32" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="50">
+      <c r="D18" s="34"/>
+      <c r="E18" s="35">
         <v>41932</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="23">
+      <c r="D19" s="29"/>
+      <c r="E19" s="17">
         <v>41928</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="25" t="s">
         <v>109</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="23">
+      <c r="D20" s="29"/>
+      <c r="E20" s="17">
         <v>41928</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26" t="s">
+      <c r="B21" s="19"/>
+      <c r="C21" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="29">
+      <c r="D21" s="20"/>
+      <c r="E21" s="23">
         <v>41928</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="55" t="s">
+      <c r="A22" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28" t="s">
+      <c r="B22" s="21"/>
+      <c r="C22" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29">
+      <c r="D22" s="22"/>
+      <c r="E22" s="23">
         <v>41934</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="25" t="s">
         <v>118</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="36" t="s">
+      <c r="C23" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="23">
+      <c r="D23" s="29"/>
+      <c r="E23" s="17">
         <v>41928</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="25" t="s">
         <v>111</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="36"/>
-      <c r="E24" s="23">
+      <c r="D24" s="29"/>
+      <c r="E24" s="17">
         <v>41928</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="25" t="s">
         <v>114</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -2144,12 +2278,12 @@
         <v>115</v>
       </c>
       <c r="D25" s="3"/>
-      <c r="E25" s="23">
+      <c r="E25" s="17">
         <v>41928</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="25" t="s">
         <v>118</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -2159,27 +2293,27 @@
         <v>117</v>
       </c>
       <c r="D26" s="4"/>
-      <c r="E26" s="23">
+      <c r="E26" s="17">
         <v>41928</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D27" s="37"/>
-      <c r="E27" s="33">
+      <c r="D27" s="30"/>
+      <c r="E27" s="26">
         <v>41928</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="25" t="s">
         <v>128</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -2189,7 +2323,7 @@
         <v>129</v>
       </c>
       <c r="D28" s="4"/>
-      <c r="E28" s="23">
+      <c r="E28" s="17">
         <v>41932</v>
       </c>
     </row>
@@ -2204,30 +2338,174 @@
         <v>138</v>
       </c>
       <c r="D29" s="3"/>
-      <c r="E29" s="23">
+      <c r="E29" s="17">
         <v>41934</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="22" t="s">
+        <v>141</v>
+      </c>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+      <c r="E30" s="23">
+        <v>41934</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" s="18"/>
+      <c r="C31" s="22" t="s">
+        <v>142</v>
+      </c>
       <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="E31" s="23">
+        <v>41935</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="84" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32" s="85"/>
+      <c r="C32" s="86" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="87"/>
+      <c r="E32" s="88">
+        <v>41935</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="40"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="23"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="40"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="23"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="40"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="23"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="79"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="83"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="79"/>
+      <c r="B37" s="80"/>
+      <c r="C37" s="81"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="83"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="79"/>
+      <c r="B38" s="80"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="83"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="74"/>
+      <c r="B39" s="75"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="78"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="54"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="53"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="59"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="58"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="54"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="53"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="54"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="56"/>
+      <c r="E43" s="53"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="59"/>
+      <c r="B44" s="73"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="58"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="54"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="53"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="54"/>
+      <c r="B46" s="52"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="53"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="59"/>
+      <c r="B47" s="73"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="58"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="54"/>
+      <c r="B48" s="52"/>
+      <c r="C48" s="55"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="53"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="54"/>
+      <c r="B49" s="52"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="53"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="59"/>
+      <c r="B50" s="73"/>
+      <c r="C50" s="60"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2242,8 +2520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2255,308 +2533,310 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="72" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="61" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="61" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="61" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="32" t="s">
+      <c r="A5" s="61"/>
+      <c r="B5" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="61" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="61" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="18" t="s">
+      <c r="B7" s="66"/>
+      <c r="C7" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="65" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="18" t="s">
+      <c r="B8" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="61" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="18" t="s">
+      <c r="B9" s="66"/>
+      <c r="C9" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="65" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="61" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="61" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="61" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="61" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="61" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="68" t="s">
         <v>134</v>
       </c>
-      <c r="D15" s="44">
+      <c r="D15" s="69">
         <v>41932</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="41"/>
+      <c r="A16" s="70"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="70"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="A17" s="70"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
     </row>
     <row r="20" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="A20" s="70"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
+      <c r="A21" s="70"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
+      <c r="A22" s="70"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
+      <c r="A23" s="70"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="A24" s="70"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
+      <c r="A25" s="70"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="70"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
+      <c r="A26" s="70"/>
+      <c r="B26" s="70"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
+      <c r="A27" s="70"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
+      <c r="A28" s="70"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
+      <c r="A29" s="70"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="70"/>
+      <c r="D29" s="70"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
+      <c r="A30" s="70"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="70"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
+      <c r="A31" s="70"/>
+      <c r="B31" s="70"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="70"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
+      <c r="A32" s="70"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2668,7 +2948,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="16" t="s">
         <v>104</v>
       </c>
       <c r="B3" t="s">

</xml_diff>

<commit_message>
versione stabile da testare 27 ottobre
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -1170,33 +1170,6 @@
     <xf numFmtId="14" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="12" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1264,6 +1237,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="12" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1697,18 +1697,18 @@
       <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="45"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="82"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1717,16 +1717,16 @@
       <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="46"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="48"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="85"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1735,16 +1735,16 @@
       <c r="B4" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="48"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="84"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="84"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="85"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1753,16 +1753,16 @@
       <c r="B5" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="48"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="85"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1771,16 +1771,16 @@
       <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="46"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="48"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="84"/>
+      <c r="P6" s="84"/>
+      <c r="Q6" s="85"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1789,16 +1789,16 @@
       <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="49"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="51"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="88"/>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1908,7 +1908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -2369,15 +2369,15 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="84" t="s">
+      <c r="A32" s="75" t="s">
         <v>143</v>
       </c>
-      <c r="B32" s="85"/>
-      <c r="C32" s="86" t="s">
+      <c r="B32" s="76"/>
+      <c r="C32" s="77" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="87"/>
-      <c r="E32" s="88">
+      <c r="D32" s="78"/>
+      <c r="E32" s="79">
         <v>41935</v>
       </c>
     </row>
@@ -2403,109 +2403,109 @@
       <c r="E35" s="23"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="79"/>
-      <c r="B36" s="80"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="82"/>
-      <c r="E36" s="83"/>
+      <c r="A36" s="70"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="74"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="79"/>
-      <c r="B37" s="80"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="82"/>
-      <c r="E37" s="83"/>
+      <c r="A37" s="70"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="74"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="79"/>
-      <c r="B38" s="80"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="83"/>
+      <c r="A38" s="70"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="74"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="74"/>
-      <c r="B39" s="75"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="77"/>
-      <c r="E39" s="78"/>
+      <c r="A39" s="65"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="69"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="54"/>
-      <c r="B40" s="52"/>
-      <c r="C40" s="55"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="53"/>
+      <c r="A40" s="45"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="44"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="59"/>
-      <c r="B41" s="73"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="58"/>
+      <c r="A41" s="50"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="49"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="54"/>
-      <c r="B42" s="52"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="53"/>
+      <c r="A42" s="45"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="44"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="54"/>
-      <c r="B43" s="52"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="56"/>
-      <c r="E43" s="53"/>
+      <c r="A43" s="45"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="44"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="59"/>
-      <c r="B44" s="73"/>
-      <c r="C44" s="60"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="58"/>
+      <c r="A44" s="50"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="49"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="54"/>
-      <c r="B45" s="52"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="53"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="44"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="54"/>
-      <c r="B46" s="52"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="53"/>
+      <c r="A46" s="45"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="44"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="59"/>
-      <c r="B47" s="73"/>
-      <c r="C47" s="60"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="58"/>
+      <c r="A47" s="50"/>
+      <c r="B47" s="64"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="49"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="54"/>
-      <c r="B48" s="52"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="53"/>
+      <c r="A48" s="45"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="44"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="54"/>
-      <c r="B49" s="52"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="56"/>
-      <c r="E49" s="53"/>
+      <c r="A49" s="45"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="44"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="59"/>
-      <c r="B50" s="73"/>
-      <c r="C50" s="60"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="58"/>
+      <c r="A50" s="50"/>
+      <c r="B50" s="64"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="48"/>
+      <c r="E50" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2533,310 +2533,310 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="63" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="52" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="52" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="52" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="61" t="s">
+      <c r="D4" s="52" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="61"/>
-      <c r="B5" s="62" t="s">
+      <c r="A5" s="52"/>
+      <c r="B5" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="52" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="D6" s="52" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="67" t="s">
+      <c r="B7" s="57"/>
+      <c r="C7" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="56" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="61" t="s">
+      <c r="D8" s="52" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="67" t="s">
+      <c r="B9" s="57"/>
+      <c r="C9" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="65" t="s">
+      <c r="D9" s="56" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="52" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="61" t="s">
+      <c r="D11" s="52" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="52" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="61" t="s">
+      <c r="D13" s="52" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="63" t="s">
+      <c r="C14" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="61" t="s">
+      <c r="D14" s="52" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="59" t="s">
         <v>134</v>
       </c>
-      <c r="D15" s="69">
+      <c r="D15" s="60">
         <v>41932</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="70"/>
-      <c r="B16" s="70"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="70"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="61"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="70"/>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="70"/>
-      <c r="B18" s="70"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
+      <c r="A18" s="61"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="70"/>
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
     </row>
     <row r="20" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="70"/>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="70"/>
-      <c r="B21" s="70"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="70"/>
-      <c r="B22" s="70"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="70"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="70"/>
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="70"/>
-      <c r="B24" s="70"/>
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="70"/>
-      <c r="B25" s="70"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="70"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="70"/>
-      <c r="B26" s="70"/>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="70"/>
-      <c r="B27" s="70"/>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="70"/>
-      <c r="B28" s="70"/>
-      <c r="C28" s="70"/>
-      <c r="D28" s="70"/>
+      <c r="A28" s="61"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="70"/>
-      <c r="B29" s="70"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="70"/>
+      <c r="A29" s="61"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="70"/>
-      <c r="B30" s="70"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
+      <c r="A30" s="61"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="61"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="70"/>
-      <c r="B31" s="70"/>
-      <c r="C31" s="70"/>
-      <c r="D31" s="70"/>
+      <c r="A31" s="61"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="70"/>
-      <c r="B32" s="70"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
versione di prova per post notifications
</commit_message>
<xml_diff>
--- a/DOC/CHANGE_LOG.xlsx
+++ b/DOC/CHANGE_LOG.xlsx
@@ -1098,7 +1098,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1264,6 +1264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1909,7 +1910,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2159,7 +2160,7 @@
       <c r="C17" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="89" t="s">
         <v>135</v>
       </c>
       <c r="E17" s="23">
@@ -2508,10 +2509,13 @@
       <c r="E50" s="49"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D17" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>